<commit_message>
Cleaning up and more model training
</commit_message>
<xml_diff>
--- a/MCA_labels.xlsx
+++ b/MCA_labels.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2442CD8-829A-4ABE-B610-22D44924F21C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{21063D0F-84AF-4FB0-8529-CE705DFC576B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -403,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW70"/>
+  <dimension ref="A1:AW71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70:A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7567,7 +7567,7 @@
       </c>
     </row>
     <row r="49" spans="1:49">
-      <c r="A49">
+      <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49">
@@ -7625,13 +7625,13 @@
         <v>0</v>
       </c>
       <c r="T49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W49">
         <v>0</v>
@@ -7716,7 +7716,7 @@
       </c>
     </row>
     <row r="50" spans="1:49">
-      <c r="A50">
+      <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50">
@@ -7771,16 +7771,16 @@
         <v>0</v>
       </c>
       <c r="S50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W50">
         <v>0</v>
@@ -7865,7 +7865,7 @@
       </c>
     </row>
     <row r="51" spans="1:49">
-      <c r="A51">
+      <c r="A51" s="1">
         <v>50</v>
       </c>
       <c r="B51">
@@ -7920,13 +7920,13 @@
         <v>0</v>
       </c>
       <c r="S51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V51">
         <v>0</v>
@@ -8014,7 +8014,7 @@
       </c>
     </row>
     <row r="52" spans="1:49">
-      <c r="A52">
+      <c r="A52" s="1">
         <v>51</v>
       </c>
       <c r="B52">
@@ -8066,16 +8066,16 @@
         <v>0</v>
       </c>
       <c r="R52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V52">
         <v>0</v>
@@ -8163,7 +8163,7 @@
       </c>
     </row>
     <row r="53" spans="1:49">
-      <c r="A53">
+      <c r="A53" s="1">
         <v>52</v>
       </c>
       <c r="B53">
@@ -8218,16 +8218,16 @@
         <v>0</v>
       </c>
       <c r="S53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W53">
         <v>0</v>
@@ -8312,7 +8312,7 @@
       </c>
     </row>
     <row r="54" spans="1:49">
-      <c r="A54">
+      <c r="A54" s="1">
         <v>53</v>
       </c>
       <c r="B54">
@@ -8364,16 +8364,16 @@
         <v>0</v>
       </c>
       <c r="R54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V54">
         <v>0</v>
@@ -8461,7 +8461,7 @@
       </c>
     </row>
     <row r="55" spans="1:49">
-      <c r="A55">
+      <c r="A55" s="1">
         <v>54</v>
       </c>
       <c r="B55">
@@ -8519,13 +8519,13 @@
         <v>0</v>
       </c>
       <c r="T55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W55">
         <v>0</v>
@@ -8610,7 +8610,7 @@
       </c>
     </row>
     <row r="56" spans="1:49">
-      <c r="A56">
+      <c r="A56" s="1">
         <v>55</v>
       </c>
       <c r="B56">
@@ -8662,13 +8662,13 @@
         <v>0</v>
       </c>
       <c r="R56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U56">
         <v>0</v>
@@ -8759,7 +8759,7 @@
       </c>
     </row>
     <row r="57" spans="1:49">
-      <c r="A57">
+      <c r="A57" s="1">
         <v>56</v>
       </c>
       <c r="B57">
@@ -8817,10 +8817,10 @@
         <v>0</v>
       </c>
       <c r="T57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V57">
         <v>0</v>
@@ -8908,7 +8908,7 @@
       </c>
     </row>
     <row r="58" spans="1:49">
-      <c r="A58">
+      <c r="A58" s="1">
         <v>57</v>
       </c>
       <c r="B58">
@@ -8954,13 +8954,13 @@
         <v>0</v>
       </c>
       <c r="P58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S58">
         <v>0</v>
@@ -9057,7 +9057,7 @@
       </c>
     </row>
     <row r="59" spans="1:49">
-      <c r="A59">
+      <c r="A59" s="1">
         <v>58</v>
       </c>
       <c r="B59">
@@ -9112,16 +9112,16 @@
         <v>0</v>
       </c>
       <c r="S59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W59">
         <v>0</v>
@@ -9206,7 +9206,7 @@
       </c>
     </row>
     <row r="60" spans="1:49">
-      <c r="A60">
+      <c r="A60" s="1">
         <v>59</v>
       </c>
       <c r="B60">
@@ -9258,13 +9258,13 @@
         <v>0</v>
       </c>
       <c r="R60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U60">
         <v>0</v>
@@ -9355,7 +9355,7 @@
       </c>
     </row>
     <row r="61" spans="1:49">
-      <c r="A61">
+      <c r="A61" s="1">
         <v>60</v>
       </c>
       <c r="B61">
@@ -9413,10 +9413,10 @@
         <v>0</v>
       </c>
       <c r="T61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V61">
         <v>0</v>
@@ -9504,7 +9504,7 @@
       </c>
     </row>
     <row r="62" spans="1:49">
-      <c r="A62">
+      <c r="A62" s="1">
         <v>61</v>
       </c>
       <c r="B62">
@@ -9553,16 +9553,16 @@
         <v>0</v>
       </c>
       <c r="Q62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U62">
         <v>0</v>
@@ -9653,7 +9653,7 @@
       </c>
     </row>
     <row r="63" spans="1:49">
-      <c r="A63">
+      <c r="A63" s="1">
         <v>62</v>
       </c>
       <c r="B63">
@@ -9696,19 +9696,19 @@
         <v>0</v>
       </c>
       <c r="O63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T63">
         <v>0</v>
@@ -9802,7 +9802,7 @@
       </c>
     </row>
     <row r="64" spans="1:49">
-      <c r="A64">
+      <c r="A64" s="1">
         <v>63</v>
       </c>
       <c r="B64">
@@ -9857,16 +9857,16 @@
         <v>0</v>
       </c>
       <c r="S64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W64">
         <v>0</v>
@@ -9951,7 +9951,7 @@
       </c>
     </row>
     <row r="65" spans="1:49">
-      <c r="A65">
+      <c r="A65" s="1">
         <v>64</v>
       </c>
       <c r="B65">
@@ -10003,13 +10003,13 @@
         <v>0</v>
       </c>
       <c r="R65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U65">
         <v>0</v>
@@ -10100,7 +10100,7 @@
       </c>
     </row>
     <row r="66" spans="1:49">
-      <c r="A66">
+      <c r="A66" s="1">
         <v>65</v>
       </c>
       <c r="B66">
@@ -10155,13 +10155,13 @@
         <v>0</v>
       </c>
       <c r="S66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V66">
         <v>0</v>
@@ -10249,7 +10249,7 @@
       </c>
     </row>
     <row r="67" spans="1:49">
-      <c r="A67">
+      <c r="A67" s="1">
         <v>66</v>
       </c>
       <c r="B67">
@@ -10298,16 +10298,16 @@
         <v>0</v>
       </c>
       <c r="Q67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U67">
         <v>0</v>
@@ -10398,7 +10398,7 @@
       </c>
     </row>
     <row r="68" spans="1:49">
-      <c r="A68">
+      <c r="A68" s="1">
         <v>67</v>
       </c>
       <c r="B68">
@@ -10447,19 +10447,19 @@
         <v>0</v>
       </c>
       <c r="Q68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V68">
         <v>0</v>
@@ -10547,7 +10547,7 @@
       </c>
     </row>
     <row r="69" spans="1:49">
-      <c r="A69">
+      <c r="A69" s="1">
         <v>68</v>
       </c>
       <c r="B69">
@@ -10599,13 +10599,13 @@
         <v>0</v>
       </c>
       <c r="R69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U69">
         <v>0</v>
@@ -10696,7 +10696,7 @@
       </c>
     </row>
     <row r="70" spans="1:49">
-      <c r="A70">
+      <c r="A70" s="1">
         <v>69</v>
       </c>
       <c r="B70">
@@ -10754,16 +10754,16 @@
         <v>0</v>
       </c>
       <c r="T70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X70">
         <v>0</v>
@@ -10841,6 +10841,155 @@
         <v>0</v>
       </c>
       <c r="AW70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:49">
+      <c r="A71" s="1">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="K71">
+        <v>0</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+      <c r="M71">
+        <v>0</v>
+      </c>
+      <c r="N71">
+        <v>0</v>
+      </c>
+      <c r="O71">
+        <v>0</v>
+      </c>
+      <c r="P71">
+        <v>0</v>
+      </c>
+      <c r="Q71">
+        <v>0</v>
+      </c>
+      <c r="R71">
+        <v>0</v>
+      </c>
+      <c r="S71">
+        <v>0</v>
+      </c>
+      <c r="T71">
+        <v>0</v>
+      </c>
+      <c r="U71">
+        <v>1</v>
+      </c>
+      <c r="V71">
+        <v>1</v>
+      </c>
+      <c r="W71">
+        <v>1</v>
+      </c>
+      <c r="X71">
+        <v>1</v>
+      </c>
+      <c r="Y71">
+        <v>0</v>
+      </c>
+      <c r="Z71">
+        <v>0</v>
+      </c>
+      <c r="AA71">
+        <v>0</v>
+      </c>
+      <c r="AB71">
+        <v>0</v>
+      </c>
+      <c r="AC71">
+        <v>0</v>
+      </c>
+      <c r="AD71">
+        <v>0</v>
+      </c>
+      <c r="AE71">
+        <v>0</v>
+      </c>
+      <c r="AF71">
+        <v>0</v>
+      </c>
+      <c r="AG71">
+        <v>0</v>
+      </c>
+      <c r="AH71">
+        <v>0</v>
+      </c>
+      <c r="AI71">
+        <v>0</v>
+      </c>
+      <c r="AJ71">
+        <v>0</v>
+      </c>
+      <c r="AK71">
+        <v>0</v>
+      </c>
+      <c r="AL71">
+        <v>0</v>
+      </c>
+      <c r="AM71">
+        <v>0</v>
+      </c>
+      <c r="AN71">
+        <v>0</v>
+      </c>
+      <c r="AO71">
+        <v>0</v>
+      </c>
+      <c r="AP71">
+        <v>0</v>
+      </c>
+      <c r="AQ71">
+        <v>0</v>
+      </c>
+      <c r="AR71">
+        <v>0</v>
+      </c>
+      <c r="AS71">
+        <v>0</v>
+      </c>
+      <c r="AT71">
+        <v>0</v>
+      </c>
+      <c r="AU71">
+        <v>0</v>
+      </c>
+      <c r="AV71">
+        <v>0</v>
+      </c>
+      <c r="AW71">
         <v>0</v>
       </c>
     </row>

</xml_diff>